<commit_message>
Template V2 for emails
</commit_message>
<xml_diff>
--- a/Src/Resources/Timeline/TimeLine.xlsx
+++ b/Src/Resources/Timeline/TimeLine.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dilan.jimenez\Desktop\LappizProjects\MercaFruta\Src\Resources\Timeline\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dilan.jimenez\Desktop\LappizProjects\FrutaNet\Src\Resources\Timeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{26F4A630-986F-4583-8DB1-DEDD065E0EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22DA0754-6F3B-488D-8E70-76CC710DFCE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="15600" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="timeLine" sheetId="1" r:id="rId1"/>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1005,12 +1005,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>